<commit_message>
adding new project management report template
</commit_message>
<xml_diff>
--- a/Compute.Documents/Gantt/Trimester 2.xlsx
+++ b/Compute.Documents/Gantt/Trimester 2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17766"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Honours\Compute.Documents\Gantt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\William\Desktop\computing-honours-project\Compute.Documents\Gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1017,8 +1017,8 @@
   </sheetPr>
   <dimension ref="B1:AP31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="BJ6" sqref="BI6:BJ6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1027,7 +1027,12 @@
     <col min="2" max="2" width="39.625" style="2" customWidth="1"/>
     <col min="3" max="6" width="11.625" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.625" style="4" customWidth="1"/>
-    <col min="8" max="27" width="2.75" style="1"/>
+    <col min="8" max="16" width="2.75" style="1"/>
+    <col min="17" max="18" width="4.375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="3.875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="4.875" style="1" customWidth="1"/>
+    <col min="21" max="27" width="2.75" style="1"/>
+    <col min="42" max="42" width="2.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:42" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1051,7 +1056,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="15">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="J3" s="16"/>
       <c r="K3" s="30" t="s">
@@ -1204,13 +1209,13 @@
         <v>3</v>
       </c>
       <c r="E6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G6" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6"/>
       <c r="V6"/>
@@ -1231,13 +1236,13 @@
         <v>3</v>
       </c>
       <c r="E7" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F7" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7"/>
       <c r="V7"/>
@@ -1258,13 +1263,13 @@
         <v>5</v>
       </c>
       <c r="E8" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G8" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8"/>
       <c r="V8"/>
@@ -1285,13 +1290,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9"/>
       <c r="V9"/>
@@ -1312,13 +1317,13 @@
         <v>8</v>
       </c>
       <c r="E10" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F10" s="7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G10" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U10"/>
       <c r="V10"/>
@@ -1339,13 +1344,13 @@
         <v>8</v>
       </c>
       <c r="E11" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G11" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11"/>
       <c r="V11"/>
@@ -1366,13 +1371,13 @@
         <v>2</v>
       </c>
       <c r="E12" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U12"/>
       <c r="V12"/>
@@ -1393,13 +1398,13 @@
         <v>4</v>
       </c>
       <c r="E13" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F13" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G13" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U13"/>
       <c r="V13"/>
@@ -1420,13 +1425,13 @@
         <v>2</v>
       </c>
       <c r="E14" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F14" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G14" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14"/>
       <c r="V14"/>
@@ -1447,13 +1452,13 @@
         <v>2</v>
       </c>
       <c r="E15" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F15" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U15"/>
       <c r="V15"/>
@@ -1474,13 +1479,13 @@
         <v>2</v>
       </c>
       <c r="E16" s="7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F16" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G16" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U16"/>
       <c r="V16"/>
@@ -1501,13 +1506,13 @@
         <v>2</v>
       </c>
       <c r="E17" s="7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F17" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G17" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U17"/>
       <c r="V17"/>
@@ -1528,13 +1533,13 @@
         <v>2</v>
       </c>
       <c r="E18" s="7">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F18" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G18" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U18"/>
       <c r="V18"/>
@@ -1555,13 +1560,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="7">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F19" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G19" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U19"/>
       <c r="V19"/>
@@ -1582,13 +1587,13 @@
         <v>2</v>
       </c>
       <c r="E20" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F20" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G20" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U20"/>
       <c r="V20"/>
@@ -1609,13 +1614,13 @@
         <v>2</v>
       </c>
       <c r="E21" s="7">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F21" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G21" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U21"/>
       <c r="V21"/>

</xml_diff>